<commit_message>
xAI modifications and slight modifs and robustness checks
</commit_message>
<xml_diff>
--- a/doc/topol_metrics_summary.xlsx
+++ b/doc/topol_metrics_summary.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tig1/Programming/TOPOL/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5EAEB-847D-2143-9B43-DF2F85976A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA25E69-0912-3148-91B4-4F25AF36E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45860" yWindow="500" windowWidth="22940" windowHeight="28300" xr2:uid="{B2B7E7B8-CE41-B34D-94A3-AE2131BD1556}"/>
+    <workbookView xWindow="22920" yWindow="500" windowWidth="45880" windowHeight="28300" activeTab="3" xr2:uid="{B2B7E7B8-CE41-B34D-94A3-AE2131BD1556}"/>
   </bookViews>
   <sheets>
     <sheet name="US Speeches" sheetId="1" r:id="rId1"/>
     <sheet name="Amazon Reviews" sheetId="2" r:id="rId2"/>
+    <sheet name="Robustness Checks" sheetId="4" r:id="rId3"/>
+    <sheet name="xAI Reporting" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="51">
   <si>
     <t>Proposed Contextual Boundary</t>
   </si>
@@ -445,6 +447,66 @@
   </si>
   <si>
     <t>p-value = (1+#{T_norm(i) ≥ T_norm(obs)}) / (1 + N_sim), where T_norm is the average drift magnitude</t>
+  </si>
+  <si>
+    <t>Robustness Check 1</t>
+  </si>
+  <si>
+    <t>Robustness Check 2</t>
+  </si>
+  <si>
+    <t>Robustness Check 3</t>
+  </si>
+  <si>
+    <t>Random CB</t>
+  </si>
+  <si>
+    <t>Drift Magnitudes</t>
+  </si>
+  <si>
+    <t>Drift Pairwise Cosine Similarity</t>
+  </si>
+  <si>
+    <t>U.S. Central Banker Speeches</t>
+  </si>
+  <si>
+    <t>Default Analysis</t>
+  </si>
+  <si>
+    <t>Amazon Reviews</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>Default CB</t>
+  </si>
+  <si>
+    <t>Generation time (minutes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average number of detected dimensions</t>
+  </si>
+  <si>
+    <t>Average number of representing sentences</t>
+  </si>
+  <si>
+    <t>Average number of contradicting sentences</t>
+  </si>
+  <si>
+    <t>Average total number of sentences</t>
+  </si>
+  <si>
+    <t>Number of clusters</t>
+  </si>
+  <si>
+    <t>Number of not empty detected dimensions</t>
   </si>
 </sst>
 </file>
@@ -541,7 +603,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -845,11 +907,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -903,6 +1070,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -921,64 +1125,95 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297343A3-4D79-AF43-AB47-4DB965BE940D}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1334,22 +1569,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="13" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="39"/>
+      <c r="F1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" s="15" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
@@ -1382,22 +1617,22 @@
       <c r="A3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="31" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1406,19 +1641,19 @@
       <c r="B4" s="29">
         <v>1.79</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="29">
         <v>1.88</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="29">
         <v>1.92</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="29">
         <v>1.88</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -1427,666 +1662,677 @@
       <c r="B5" s="29">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="29">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="29">
         <v>0.51</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="29">
         <v>0.47</v>
       </c>
-      <c r="I5" s="34"/>
-    </row>
-    <row r="6" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="35" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="35" t="s">
+      <c r="G8" s="32"/>
+      <c r="H8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="36"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.61</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.16</v>
-      </c>
+      <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3">
-        <v>0.53</v>
+        <v>0.61</v>
       </c>
       <c r="C9" s="1">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="D9" s="3">
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
       <c r="E9" s="1">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="F9" s="3">
-        <v>0.52</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G9" s="1">
-        <v>0.53</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H9" s="2">
-        <v>0.55000000000000004</v>
+        <v>0.63</v>
       </c>
       <c r="I9" s="5">
-        <v>0.54</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="C10" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="D10" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
       <c r="E10" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="F10" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
       <c r="G10" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="H10" s="2">
-        <v>0.31</v>
+        <v>0.17</v>
       </c>
       <c r="I10" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
       <c r="C11" s="1">
-        <v>0.02</v>
+        <v>0.53</v>
       </c>
       <c r="D11" s="3">
-        <v>0.08</v>
+        <v>0.52</v>
       </c>
       <c r="E11" s="1">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
       <c r="F11" s="3">
-        <v>0.08</v>
+        <v>0.52</v>
       </c>
       <c r="G11" s="1">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
       <c r="H11" s="2">
-        <v>0.05</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I11" s="5">
-        <v>0.03</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3">
-        <v>-0.01</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C12" s="1">
-        <v>0.02</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E12" s="1">
-        <v>0.03</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H12" s="2">
-        <v>-0.01</v>
+        <v>0.31</v>
       </c>
       <c r="I12" s="5">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="C13" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D13" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E13" s="1">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F13" s="3">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="G13" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H13" s="2">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="I13" s="5">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>0.08</v>
+        <v>-0.01</v>
       </c>
       <c r="C14" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="D14" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0.03</v>
       </c>
       <c r="F14" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0.08</v>
+        <v>-0.01</v>
       </c>
       <c r="I14" s="5">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="F15" s="3">
         <v>0.1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="G15" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F16" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G16" s="1">
         <v>0.04</v>
       </c>
-      <c r="D15" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="36"/>
+      <c r="H16" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="C17" s="1">
-        <v>0.61</v>
+        <v>0.04</v>
       </c>
       <c r="D17" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.09</v>
       </c>
       <c r="E17" s="1">
-        <v>0.61</v>
+        <v>0.06</v>
       </c>
       <c r="F17" s="3">
-        <v>0.53</v>
+        <v>0.11</v>
       </c>
       <c r="G17" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.06</v>
       </c>
       <c r="H17" s="2">
-        <v>0.62</v>
+        <v>0.1</v>
       </c>
       <c r="I17" s="5">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0.17</v>
-      </c>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="43"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="3">
-        <v>0.52</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C19" s="1">
-        <v>0.54</v>
+        <v>0.61</v>
       </c>
       <c r="D19" s="3">
-        <v>0.5</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E19" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="F19" s="3">
         <v>0.53</v>
       </c>
-      <c r="F19" s="3">
-        <v>0.5</v>
-      </c>
       <c r="G19" s="1">
-        <v>0.53</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H19" s="2">
-        <v>0.52</v>
+        <v>0.62</v>
       </c>
       <c r="I19" s="5">
-        <v>0.55000000000000004</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
       <c r="C20" s="1">
-        <v>0.3</v>
+        <v>0.16</v>
       </c>
       <c r="D20" s="3">
-        <v>0.26</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E20" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="F20" s="3">
-        <v>0.26</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G20" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
       <c r="H20" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.15</v>
       </c>
       <c r="I20" s="5">
-        <v>0.31</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2">
-        <v>-0.02</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.52</v>
       </c>
       <c r="C21" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
+        <v>0.54</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.5</v>
       </c>
       <c r="E21" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
+        <v>0.53</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.5</v>
       </c>
       <c r="G21" s="1">
-        <v>0.04</v>
+        <v>0.53</v>
       </c>
       <c r="H21" s="2">
-        <v>0.04</v>
+        <v>0.52</v>
       </c>
       <c r="I21" s="5">
-        <v>0.01</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.04</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.28000000000000003</v>
       </c>
       <c r="C22" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.04</v>
+        <v>0.3</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.26</v>
       </c>
       <c r="E22" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.02</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.26</v>
       </c>
       <c r="G22" s="1">
-        <v>0.01</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H22" s="2">
-        <v>0.03</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I22" s="5">
-        <v>0</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2">
-        <v>0.06</v>
+        <v>-0.02</v>
       </c>
       <c r="C23" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.09</v>
-      </c>
       <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
         <v>0.04</v>
       </c>
-      <c r="G23" s="1">
-        <v>0.08</v>
-      </c>
       <c r="H23" s="2">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="I23" s="5">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B26" s="3">
         <v>0</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <v>0.03</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D26" s="3">
         <v>0</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E26" s="1">
         <v>0.03</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G26" s="1">
         <v>0.03</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H26" s="2">
         <v>-0.03</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I26" s="5">
         <v>0.03</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="27" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B27" s="8">
         <v>0.04</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C27" s="9">
         <v>0.06</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D27" s="8">
         <v>0.06</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E27" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F27" s="8">
         <v>0.06</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G27" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H27" s="10">
         <v>0.01</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I27" s="11">
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" s="22" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="24"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" ht="22" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
+    <row r="31" spans="1:9" s="22" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="37"/>
+      <c r="H31" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="37"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B34" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45" t="s">
+      <c r="C34" s="47"/>
+      <c r="D34" s="48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="40" t="s">
+    <row r="35" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="27"/>
+      <c r="B35" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C35" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D35" s="23">
         <v>9.990000000000001E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="42">
+    <row r="36" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="25">
         <v>0.12</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C36" s="11">
         <v>0</v>
       </c>
-      <c r="D34" s="39"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="D36" s="24"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
@@ -2095,6 +2341,9 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
@@ -2172,26 +2421,16 @@
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -2200,10 +2439,28 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2215,7 +2472,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2233,22 +2490,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="13" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="39"/>
+      <c r="F1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" s="15" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
@@ -2281,22 +2538,22 @@
       <c r="A3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="31" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2305,19 +2562,19 @@
       <c r="B4" s="29">
         <v>4.42</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="29">
         <v>4.6500000000000004</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="29">
         <v>4.58</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="29">
         <v>5.12</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -2326,40 +2583,40 @@
       <c r="B5" s="29">
         <v>1.6</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="29">
         <v>1.48</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="29">
         <v>1.54</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="29">
         <v>1.53</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
@@ -2626,22 +2883,22 @@
       <c r="A16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="35" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="35" t="s">
+      <c r="E16" s="32"/>
+      <c r="F16" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="35" t="s">
+      <c r="G16" s="32"/>
+      <c r="H16" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="36"/>
+      <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
@@ -2917,57 +3174,57 @@
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:9" s="22" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="23" t="s">
+      <c r="C29" s="37"/>
+      <c r="D29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="23" t="s">
+      <c r="E29" s="37"/>
+      <c r="F29" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="23" t="s">
+      <c r="G29" s="37"/>
+      <c r="H29" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="24"/>
+      <c r="I29" s="37"/>
     </row>
     <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" ht="22" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
+    <row r="32" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45" t="s">
+      <c r="C32" s="47"/>
+      <c r="D32" s="48" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="23">
         <v>9.990000000000001E-4</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="42">
+      <c r="A34" s="28"/>
+      <c r="B34" s="25">
         <v>0.66</v>
       </c>
       <c r="C34" s="11">
         <v>0</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="24"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
@@ -2986,12 +3243,18 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -3000,22 +3263,740 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3CE3D4-8BBE-4A48-851B-E4950C6B2F5F}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="49"/>
+      <c r="B1" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+      <c r="B2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="67"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="52">
+        <v>0.13</v>
+      </c>
+      <c r="C5" s="53">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D5" s="54">
+        <v>0.43</v>
+      </c>
+      <c r="E5" s="52">
+        <v>-0.09</v>
+      </c>
+      <c r="F5" s="70">
+        <v>0.12</v>
+      </c>
+      <c r="G5" s="54">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="52">
+        <v>0.11</v>
+      </c>
+      <c r="C6" s="53">
+        <v>0.17</v>
+      </c>
+      <c r="D6" s="54">
+        <v>0.23</v>
+      </c>
+      <c r="E6" s="52">
+        <v>-0.2</v>
+      </c>
+      <c r="F6" s="70">
+        <v>-0.01</v>
+      </c>
+      <c r="G6" s="54">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="54"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="52">
+        <v>0.13</v>
+      </c>
+      <c r="C8" s="53">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="54">
+        <v>0.43</v>
+      </c>
+      <c r="E8" s="52">
+        <v>-0.09</v>
+      </c>
+      <c r="F8" s="70">
+        <v>0.13</v>
+      </c>
+      <c r="G8" s="54">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="52">
+        <v>0.11</v>
+      </c>
+      <c r="C9" s="70">
+        <v>0.17</v>
+      </c>
+      <c r="D9" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="52">
+        <v>-0.26</v>
+      </c>
+      <c r="F9" s="70">
+        <v>-0.01</v>
+      </c>
+      <c r="G9" s="54">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="54"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="52">
+        <v>0.12</v>
+      </c>
+      <c r="C11" s="70">
+        <v>0.32</v>
+      </c>
+      <c r="D11" s="54">
+        <v>0.54</v>
+      </c>
+      <c r="E11" s="52">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="F11" s="70">
+        <v>0.11</v>
+      </c>
+      <c r="G11" s="54">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="52">
+        <v>0.11</v>
+      </c>
+      <c r="C12" s="70">
+        <v>0.17</v>
+      </c>
+      <c r="D12" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="52">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="F12" s="70">
+        <v>0</v>
+      </c>
+      <c r="G12" s="54">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="52">
+        <v>0.13</v>
+      </c>
+      <c r="C14" s="70">
+        <v>0.26</v>
+      </c>
+      <c r="D14" s="54">
+        <v>0.35</v>
+      </c>
+      <c r="E14" s="52">
+        <v>-0.16</v>
+      </c>
+      <c r="F14" s="70">
+        <v>0.19</v>
+      </c>
+      <c r="G14" s="54">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="52">
+        <v>0.11</v>
+      </c>
+      <c r="C15" s="70">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D15" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="E15" s="52">
+        <v>-0.15</v>
+      </c>
+      <c r="F15" s="70">
+        <v>0</v>
+      </c>
+      <c r="G15" s="54">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="52">
+        <v>0.21</v>
+      </c>
+      <c r="C18" s="53">
+        <v>0.33</v>
+      </c>
+      <c r="D18" s="54">
+        <v>0.49</v>
+      </c>
+      <c r="E18" s="52">
+        <v>0.21</v>
+      </c>
+      <c r="F18" s="70">
+        <v>0.66</v>
+      </c>
+      <c r="G18" s="54">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="52">
+        <v>0.04</v>
+      </c>
+      <c r="C19" s="53">
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="54">
+        <v>0.12</v>
+      </c>
+      <c r="E19" s="52">
+        <v>-0.15</v>
+      </c>
+      <c r="F19" s="70">
+        <v>0</v>
+      </c>
+      <c r="G19" s="54">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="52">
+        <v>0.21</v>
+      </c>
+      <c r="C21" s="53">
+        <v>0.33</v>
+      </c>
+      <c r="D21" s="54">
+        <v>0.59</v>
+      </c>
+      <c r="E21" s="52">
+        <v>0.24</v>
+      </c>
+      <c r="F21" s="70">
+        <v>0.65</v>
+      </c>
+      <c r="G21" s="54">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="52">
+        <v>0.04</v>
+      </c>
+      <c r="C22" s="70">
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="54">
+        <v>0.13</v>
+      </c>
+      <c r="E22" s="52">
+        <v>-0.15</v>
+      </c>
+      <c r="F22" s="70">
+        <v>0</v>
+      </c>
+      <c r="G22" s="54">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="52">
+        <v>0.24</v>
+      </c>
+      <c r="C24" s="70">
+        <v>0.33</v>
+      </c>
+      <c r="D24" s="54">
+        <v>0.51</v>
+      </c>
+      <c r="E24" s="52">
+        <v>0.23</v>
+      </c>
+      <c r="F24" s="70">
+        <v>0.66</v>
+      </c>
+      <c r="G24" s="54">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="52">
+        <v>0.04</v>
+      </c>
+      <c r="C25" s="70">
+        <v>0.08</v>
+      </c>
+      <c r="D25" s="54">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E25" s="52">
+        <v>-0.15</v>
+      </c>
+      <c r="F25" s="70">
+        <v>-0.01</v>
+      </c>
+      <c r="G25" s="54">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="54"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="52">
+        <v>0.21</v>
+      </c>
+      <c r="C27" s="70">
+        <v>0.32</v>
+      </c>
+      <c r="D27" s="54">
+        <v>0.43</v>
+      </c>
+      <c r="E27" s="52">
+        <v>0.45</v>
+      </c>
+      <c r="F27" s="70">
+        <v>0.74</v>
+      </c>
+      <c r="G27" s="54">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="C28" s="58">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D28" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E28" s="60">
+        <v>-0.19</v>
+      </c>
+      <c r="F28" s="58">
+        <v>-0.01</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CE4942-BAB0-D543-BE17-4DFE57F25859}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54.1640625" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="49"/>
+      <c r="B1" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="59">
+        <v>11</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="59">
+        <v>15</v>
+      </c>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="72">
+        <v>47</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="71">
+        <v>43</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="72">
+        <v>7</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="71">
+        <v>6</v>
+      </c>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="72"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="78"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>